<commit_message>
Fix direction of treatment support effect
</commit_message>
<xml_diff>
--- a/tests/databooks/progbook_tb_simple.xlsx
+++ b/tests/databooks/progbook_tb_simple.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robynstuart/Documents/git/atomica/tests/databooks/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\atomica\atomica\tests\databooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{5206528C-363F-3943-8516-1DA13EC44550}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7798971F-E39F-4064-9E06-7A6F0AF3282A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="25360" windowHeight="9660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="465" windowWidth="25365" windowHeight="9660" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Program targeting" sheetId="1" r:id="rId1"/>
@@ -19,8 +19,16 @@
   </sheets>
   <externalReferences>
     <externalReference r:id="rId4"/>
+    <externalReference r:id="rId5"/>
   </externalReferences>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -285,367 +293,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="112">
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <bgColor rgb="FFEEEEEE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFCCCCCC"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFCCCCCC"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFCCCCCC"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFCCCCCC"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <bgColor rgb="FFEEEEEE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFCCCCCC"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFCCCCCC"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFCCCCCC"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFCCCCCC"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <bgColor rgb="FFEEEEEE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFCCCCCC"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFCCCCCC"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFCCCCCC"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFCCCCCC"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <bgColor rgb="FFEEEEEE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFCCCCCC"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFCCCCCC"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFCCCCCC"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFCCCCCC"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <bgColor rgb="FFEEEEEE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFCCCCCC"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFCCCCCC"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFCCCCCC"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFCCCCCC"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <bgColor rgb="FFEEEEEE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFCCCCCC"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFCCCCCC"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFCCCCCC"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFCCCCCC"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <bgColor rgb="FFEEEEEE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFCCCCCC"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFCCCCCC"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFCCCCCC"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFCCCCCC"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <bgColor rgb="FFEEEEEE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFCCCCCC"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFCCCCCC"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFCCCCCC"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFCCCCCC"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <bgColor rgb="FFEEEEEE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFCCCCCC"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFCCCCCC"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFCCCCCC"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFCCCCCC"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <bgColor rgb="FFEEEEEE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFCCCCCC"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFCCCCCC"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFCCCCCC"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFCCCCCC"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <bgColor rgb="FFEEEEEE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFCCCCCC"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFCCCCCC"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFCCCCCC"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFCCCCCC"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <bgColor rgb="FFEEEEEE"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color rgb="FFCCCCCC"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFCCCCCC"/>
-        </right>
-        <top style="thin">
-          <color rgb="FFCCCCCC"/>
-        </top>
-        <bottom style="thin">
-          <color rgb="FFCCCCCC"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="lightUp">
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="88">
     <dxf>
       <fill>
         <patternFill patternType="lightUp">
@@ -1450,6 +1098,19 @@
       </sheetData>
       <sheetData sheetId="1"/>
       <sheetData sheetId="2"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Program targeting"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1782,13 +1443,13 @@
       <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="14.83203125" customWidth="1"/>
-    <col min="5" max="9" width="14.83203125" customWidth="1"/>
+    <col min="1" max="3" width="14.85546875" customWidth="1"/>
+    <col min="5" max="9" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1796,7 +1457,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
@@ -1822,7 +1483,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -1848,7 +1509,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -1874,7 +1535,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>27</v>
       </c>
@@ -1900,7 +1561,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>28</v>
       </c>
@@ -1928,122 +1589,122 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C3:C6">
-    <cfRule type="cellIs" dxfId="111" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="87" priority="1" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
-    <cfRule type="cellIs" dxfId="110" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="86" priority="7" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="cellIs" dxfId="109" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="85" priority="13" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6">
-    <cfRule type="cellIs" dxfId="108" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="84" priority="19" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="cellIs" dxfId="107" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="83" priority="2" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4">
-    <cfRule type="cellIs" dxfId="106" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="82" priority="8" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="cellIs" dxfId="105" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="81" priority="14" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="104" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="80" priority="20" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3">
-    <cfRule type="cellIs" dxfId="103" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="79" priority="3" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4">
-    <cfRule type="cellIs" dxfId="102" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="78" priority="9" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="cellIs" dxfId="101" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="15" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F6">
-    <cfRule type="cellIs" dxfId="100" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="21" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3">
-    <cfRule type="cellIs" dxfId="99" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="4" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4">
-    <cfRule type="cellIs" dxfId="98" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="10" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5">
-    <cfRule type="cellIs" dxfId="97" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="16" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G6">
-    <cfRule type="cellIs" dxfId="96" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="22" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H3">
-    <cfRule type="cellIs" dxfId="95" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="71" priority="5" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H4">
-    <cfRule type="cellIs" dxfId="94" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="70" priority="11" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="cellIs" dxfId="93" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="69" priority="17" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6">
-    <cfRule type="cellIs" dxfId="92" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="68" priority="23" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3">
-    <cfRule type="cellIs" dxfId="91" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="67" priority="6" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4">
-    <cfRule type="cellIs" dxfId="90" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="66" priority="12" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" dxfId="89" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="65" priority="18" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6">
-    <cfRule type="cellIs" dxfId="88" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="64" priority="24" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2060,20 +1721,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.83203125" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" customWidth="1"/>
-    <col min="4" max="4" width="3.83203125" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="3.85546875" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="str">
         <f>'Program targeting'!$A$3</f>
         <v>Passive case finding</v>
@@ -2101,7 +1762,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>13</v>
       </c>
@@ -2118,7 +1779,7 @@
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
@@ -2136,7 +1797,7 @@
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
@@ -2151,7 +1812,7 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
@@ -2166,7 +1827,7 @@
       <c r="H5" s="5"/>
       <c r="I5" s="5"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
@@ -2183,7 +1844,7 @@
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="str">
         <f>'Program targeting'!$A$4</f>
         <v>Active case finding</v>
@@ -2211,7 +1872,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
@@ -2228,7 +1889,7 @@
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -2246,7 +1907,7 @@
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
@@ -2261,7 +1922,7 @@
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
@@ -2276,7 +1937,7 @@
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
@@ -2293,7 +1954,7 @@
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="str">
         <f>'Program targeting'!$A$5</f>
         <v>Treatment initiation</v>
@@ -2321,7 +1982,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
@@ -2338,7 +1999,7 @@
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
@@ -2355,7 +2016,7 @@
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
@@ -2370,7 +2031,7 @@
       <c r="H18" s="5"/>
       <c r="I18" s="5"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
@@ -2385,7 +2046,7 @@
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
@@ -2402,7 +2063,7 @@
       <c r="H20" s="5"/>
       <c r="I20" s="5"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="str">
         <f>'Program targeting'!$A$6</f>
         <v>Treatment support</v>
@@ -2430,7 +2091,7 @@
         <v>2018</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>13</v>
       </c>
@@ -2447,7 +2108,7 @@
       <c r="H23" s="5"/>
       <c r="I23" s="5"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>15</v>
       </c>
@@ -2464,7 +2125,7 @@
       <c r="H24" s="5"/>
       <c r="I24" s="5"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>16</v>
       </c>
@@ -2479,7 +2140,7 @@
       <c r="H25" s="5"/>
       <c r="I25" s="5"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>17</v>
       </c>
@@ -2494,7 +2155,7 @@
       <c r="H26" s="5"/>
       <c r="I26" s="5"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>18</v>
       </c>
@@ -2513,162 +2174,162 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C10">
-    <cfRule type="expression" dxfId="87" priority="13">
+    <cfRule type="expression" dxfId="63" priority="13">
       <formula>COUNTIF(E10:I10,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="86" priority="14">
+    <cfRule type="expression" dxfId="62" priority="14">
       <formula>AND(COUNTIF(E10:I10,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C10)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C11">
-    <cfRule type="expression" dxfId="85" priority="15">
+    <cfRule type="expression" dxfId="61" priority="15">
       <formula>COUNTIF(E11:I11,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="84" priority="16">
+    <cfRule type="expression" dxfId="60" priority="16">
       <formula>AND(COUNTIF(E11:I11,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C11)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C12">
-    <cfRule type="expression" dxfId="83" priority="17">
+    <cfRule type="expression" dxfId="59" priority="17">
       <formula>COUNTIF(E12:I12,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="82" priority="18">
+    <cfRule type="expression" dxfId="58" priority="18">
       <formula>AND(COUNTIF(E12:I12,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C12)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C13">
-    <cfRule type="expression" dxfId="81" priority="19">
+    <cfRule type="expression" dxfId="57" priority="19">
       <formula>COUNTIF(E13:I13,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="80" priority="20">
+    <cfRule type="expression" dxfId="56" priority="20">
       <formula>AND(COUNTIF(E13:I13,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C13)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C16">
-    <cfRule type="expression" dxfId="79" priority="21">
+    <cfRule type="expression" dxfId="55" priority="21">
       <formula>COUNTIF(E16:I16,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="78" priority="22">
+    <cfRule type="expression" dxfId="54" priority="22">
       <formula>AND(COUNTIF(E16:I16,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C17">
-    <cfRule type="expression" dxfId="77" priority="23">
+    <cfRule type="expression" dxfId="53" priority="23">
       <formula>COUNTIF(E17:I17,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="76" priority="24">
+    <cfRule type="expression" dxfId="52" priority="24">
       <formula>AND(COUNTIF(E17:I17,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C17)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18">
-    <cfRule type="expression" dxfId="75" priority="25">
+    <cfRule type="expression" dxfId="51" priority="25">
       <formula>COUNTIF(E18:I18,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="74" priority="26">
+    <cfRule type="expression" dxfId="50" priority="26">
       <formula>AND(COUNTIF(E18:I18,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C18)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C19">
-    <cfRule type="expression" dxfId="73" priority="27">
+    <cfRule type="expression" dxfId="49" priority="27">
       <formula>COUNTIF(E19:I19,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="72" priority="28">
+    <cfRule type="expression" dxfId="48" priority="28">
       <formula>AND(COUNTIF(E19:I19,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C19)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2">
-    <cfRule type="expression" dxfId="71" priority="1">
+    <cfRule type="expression" dxfId="47" priority="1">
       <formula>COUNTIF(E2:I2,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="70" priority="2">
+    <cfRule type="expression" dxfId="46" priority="2">
       <formula>AND(COUNTIF(E2:I2,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20">
-    <cfRule type="expression" dxfId="69" priority="29">
+    <cfRule type="expression" dxfId="45" priority="29">
       <formula>COUNTIF(E20:I20,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="68" priority="30">
+    <cfRule type="expression" dxfId="44" priority="30">
       <formula>AND(COUNTIF(E20:I20,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C23">
-    <cfRule type="expression" dxfId="67" priority="31">
+    <cfRule type="expression" dxfId="43" priority="31">
       <formula>COUNTIF(E23:I23,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="66" priority="32">
+    <cfRule type="expression" dxfId="42" priority="32">
       <formula>AND(COUNTIF(E23:I23,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C23)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C24">
-    <cfRule type="expression" dxfId="65" priority="33">
+    <cfRule type="expression" dxfId="41" priority="33">
       <formula>COUNTIF(E24:I24,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="34">
+    <cfRule type="expression" dxfId="40" priority="34">
       <formula>AND(COUNTIF(E24:I24,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C24)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C25">
-    <cfRule type="expression" dxfId="63" priority="35">
+    <cfRule type="expression" dxfId="39" priority="35">
       <formula>COUNTIF(E25:I25,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="62" priority="36">
+    <cfRule type="expression" dxfId="38" priority="36">
       <formula>AND(COUNTIF(E25:I25,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C26">
-    <cfRule type="expression" dxfId="61" priority="37">
+    <cfRule type="expression" dxfId="37" priority="37">
       <formula>COUNTIF(E26:I26,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="38">
+    <cfRule type="expression" dxfId="36" priority="38">
       <formula>AND(COUNTIF(E26:I26,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C26)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C27">
-    <cfRule type="expression" dxfId="59" priority="39">
+    <cfRule type="expression" dxfId="35" priority="39">
       <formula>COUNTIF(E27:I27,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="40">
+    <cfRule type="expression" dxfId="34" priority="40">
       <formula>AND(COUNTIF(E27:I27,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C27)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C3">
-    <cfRule type="expression" dxfId="57" priority="3">
+    <cfRule type="expression" dxfId="33" priority="3">
       <formula>COUNTIF(E3:I3,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="56" priority="4">
+    <cfRule type="expression" dxfId="32" priority="4">
       <formula>AND(COUNTIF(E3:I3,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4">
-    <cfRule type="expression" dxfId="55" priority="5">
+    <cfRule type="expression" dxfId="31" priority="5">
       <formula>COUNTIF(E4:I4,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="6">
+    <cfRule type="expression" dxfId="30" priority="6">
       <formula>AND(COUNTIF(E4:I4,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="expression" dxfId="53" priority="7">
+    <cfRule type="expression" dxfId="29" priority="7">
       <formula>COUNTIF(E5:I5,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="52" priority="8">
+    <cfRule type="expression" dxfId="28" priority="8">
       <formula>AND(COUNTIF(E5:I5,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C6">
-    <cfRule type="expression" dxfId="51" priority="9">
+    <cfRule type="expression" dxfId="27" priority="9">
       <formula>COUNTIF(E6:I6,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="50" priority="10">
+    <cfRule type="expression" dxfId="26" priority="10">
       <formula>AND(COUNTIF(E6:I6,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C9">
-    <cfRule type="expression" dxfId="49" priority="11">
+    <cfRule type="expression" dxfId="25" priority="11">
       <formula>COUNTIF(E9:I9,"&lt;&gt;" &amp; "")&gt;0</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="12">
+    <cfRule type="expression" dxfId="24" priority="12">
       <formula>AND(COUNTIF(E9:I9,"&lt;&gt;" &amp; "")&gt;0,NOT(ISBLANK(C9)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2682,20 +2343,20 @@
   <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="103" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5:J8"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="1.5" customWidth="1"/>
-    <col min="7" max="10" width="10.83203125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="1.42578125" customWidth="1"/>
+    <col min="7" max="10" width="10.85546875" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -2728,7 +2389,7 @@
         <v>Treatment support</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>'Program targeting'!$C$2</f>
         <v>Adults</v>
@@ -2752,7 +2413,7 @@
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
     </row>
-    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>23</v>
       </c>
@@ -2785,7 +2446,7 @@
         <v>Treatment support</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>'Program targeting'!$C$2</f>
         <v>Adults</v>
@@ -2807,7 +2468,7 @@
       </c>
       <c r="J5" s="8"/>
     </row>
-    <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>24</v>
       </c>
@@ -2840,7 +2501,7 @@
         <v>Treatment support</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>'Program targeting'!$C$2</f>
         <v>Adults</v>
@@ -2859,7 +2520,7 @@
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
       <c r="J8" s="8">
-        <v>0.15</v>
+        <v>0.05</v>
       </c>
     </row>
   </sheetData>
@@ -3111,7 +2772,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="9" id="{3DC31EF4-9C03-4E4A-BE0B-5D290A41A6BA}">
-            <xm:f>AND('/Users/robynstuart/Documents/git/atomica/tests/databooks/[progbook_tb_simple_dyn.xlsx]Program targeting'!#REF!&lt;&gt;"Y",NOT(ISBLANK(G2)))</xm:f>
+            <xm:f>AND('C:\Users\robynstuart\Documents\git\atomica\tests\databooks\[progbook_tb_simple_dyn.xlsx]Program targeting'!#REF!&lt;&gt;"Y",NOT(ISBLANK(G2)))</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill patternType="lightUp">
@@ -3121,7 +2782,7 @@
             </x14:dxf>
           </x14:cfRule>
           <x14:cfRule type="expression" priority="10" id="{EC619C9F-3EA3-3E48-B43D-4372CD341D33}">
-            <xm:f>'/Users/robynstuart/Documents/git/atomica/tests/databooks/[progbook_tb_simple_dyn.xlsx]Program targeting'!#REF!&lt;&gt;"Y"</xm:f>
+            <xm:f>'C:\Users\robynstuart\Documents\git\atomica\tests\databooks\[progbook_tb_simple_dyn.xlsx]Program targeting'!#REF!&lt;&gt;"Y"</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill patternType="lightUp">
@@ -3150,7 +2811,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="11" id="{1C551198-1DF3-834C-9119-901E3F7A8A86}">
-            <xm:f>AND('/Users/robynstuart/Documents/git/atomica/tests/databooks/[progbook_tb_simple_dyn.xlsx]Program targeting'!#REF!&lt;&gt;"Y",NOT(ISBLANK(H2)))</xm:f>
+            <xm:f>AND('C:\Users\robynstuart\Documents\git\atomica\tests\databooks\[progbook_tb_simple_dyn.xlsx]Program targeting'!#REF!&lt;&gt;"Y",NOT(ISBLANK(H2)))</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill patternType="lightUp">
@@ -3160,7 +2821,7 @@
             </x14:dxf>
           </x14:cfRule>
           <x14:cfRule type="expression" priority="12" id="{612BBDFA-5A41-3E44-B530-5C830913FC23}">
-            <xm:f>'/Users/robynstuart/Documents/git/atomica/tests/databooks/[progbook_tb_simple_dyn.xlsx]Program targeting'!#REF!&lt;&gt;"Y"</xm:f>
+            <xm:f>'C:\Users\robynstuart\Documents\git\atomica\tests\databooks\[progbook_tb_simple_dyn.xlsx]Program targeting'!#REF!&lt;&gt;"Y"</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill patternType="lightUp">
@@ -3189,7 +2850,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="7" id="{1E77E578-4BAA-3043-AAC0-2B9294F3CF3E}">
-            <xm:f>AND('/Users/robynstuart/Documents/git/atomica/tests/databooks/[progbook_tb_simple_dyn.xlsx]Program targeting'!#REF!&lt;&gt;"Y",NOT(ISBLANK(I8)))</xm:f>
+            <xm:f>AND('C:\Users\robynstuart\Documents\git\atomica\tests\databooks\[progbook_tb_simple_dyn.xlsx]Program targeting'!#REF!&lt;&gt;"Y",NOT(ISBLANK(I8)))</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill patternType="lightUp">
@@ -3199,7 +2860,7 @@
             </x14:dxf>
           </x14:cfRule>
           <x14:cfRule type="expression" priority="8" id="{4B360A0F-C52D-1143-B9E2-D9988605373A}">
-            <xm:f>'/Users/robynstuart/Documents/git/atomica/tests/databooks/[progbook_tb_simple_dyn.xlsx]Program targeting'!#REF!&lt;&gt;"Y"</xm:f>
+            <xm:f>'C:\Users\robynstuart\Documents\git\atomica\tests\databooks\[progbook_tb_simple_dyn.xlsx]Program targeting'!#REF!&lt;&gt;"Y"</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill patternType="lightUp">
@@ -3228,7 +2889,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="3" id="{A790C77D-D849-AC43-A87C-0C2885D53234}">
-            <xm:f>AND('/Users/robynstuart/Documents/git/atomica/tests/databooks/[progbook_tb_simple_dyn.xlsx]Program targeting'!#REF!&lt;&gt;"Y",NOT(ISBLANK(I5)))</xm:f>
+            <xm:f>AND('C:\Users\robynstuart\Documents\git\atomica\tests\databooks\[progbook_tb_simple_dyn.xlsx]Program targeting'!#REF!&lt;&gt;"Y",NOT(ISBLANK(I5)))</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill patternType="lightUp">
@@ -3238,7 +2899,7 @@
             </x14:dxf>
           </x14:cfRule>
           <x14:cfRule type="expression" priority="4" id="{B28E66A5-A498-DE43-B017-500C955EA72D}">
-            <xm:f>'/Users/robynstuart/Documents/git/atomica/tests/databooks/[progbook_tb_simple_dyn.xlsx]Program targeting'!#REF!&lt;&gt;"Y"</xm:f>
+            <xm:f>'C:\Users\robynstuart\Documents\git\atomica\tests\databooks\[progbook_tb_simple_dyn.xlsx]Program targeting'!#REF!&lt;&gt;"Y"</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill patternType="lightUp">
@@ -3267,7 +2928,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="5" id="{3EDFEA2D-6231-5B43-8648-8AD810F0CAFB}">
-            <xm:f>AND('/Users/robynstuart/Documents/git/atomica/tests/databooks/[progbook_tb_simple_dyn.xlsx]Program targeting'!#REF!&lt;&gt;"Y",NOT(ISBLANK(J5)))</xm:f>
+            <xm:f>AND('C:\Users\robynstuart\Documents\git\atomica\tests\databooks\[progbook_tb_simple_dyn.xlsx]Program targeting'!#REF!&lt;&gt;"Y",NOT(ISBLANK(J5)))</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill patternType="lightUp">
@@ -3277,7 +2938,7 @@
             </x14:dxf>
           </x14:cfRule>
           <x14:cfRule type="expression" priority="6" id="{D1CB22EF-615E-5444-9F21-98928479B963}">
-            <xm:f>'/Users/robynstuart/Documents/git/atomica/tests/databooks/[progbook_tb_simple_dyn.xlsx]Program targeting'!#REF!&lt;&gt;"Y"</xm:f>
+            <xm:f>'C:\Users\robynstuart\Documents\git\atomica\tests\databooks\[progbook_tb_simple_dyn.xlsx]Program targeting'!#REF!&lt;&gt;"Y"</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill patternType="lightUp">
@@ -3306,7 +2967,7 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="expression" priority="1" id="{6FADB7D4-72A2-CA47-996E-BF73A7CAC581}">
-            <xm:f>AND('/Users/robynstuart/Documents/git/atomica/tests/databooks/[progbook_tb_simple_dyn.xlsx]Program targeting'!#REF!&lt;&gt;"Y",NOT(ISBLANK(J8)))</xm:f>
+            <xm:f>AND('C:\Users\robynstuart\Documents\git\atomica\tests\databooks\[progbook_tb_simple_dyn.xlsx]Program targeting'!#REF!&lt;&gt;"Y",NOT(ISBLANK(J8)))</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill patternType="lightUp">
@@ -3316,7 +2977,7 @@
             </x14:dxf>
           </x14:cfRule>
           <x14:cfRule type="expression" priority="2" id="{3B257E8C-CB74-C945-8192-91A3B44230D2}">
-            <xm:f>'/Users/robynstuart/Documents/git/atomica/tests/databooks/[progbook_tb_simple_dyn.xlsx]Program targeting'!#REF!&lt;&gt;"Y"</xm:f>
+            <xm:f>'C:\Users\robynstuart\Documents\git\atomica\tests\databooks\[progbook_tb_simple_dyn.xlsx]Program targeting'!#REF!&lt;&gt;"Y"</xm:f>
             <x14:dxf>
               <fill>
                 <patternFill patternType="lightUp">

</xml_diff>